<commit_message>
Removed permanent cell address in excel template formulae
</commit_message>
<xml_diff>
--- a/src/Input/MasterTemplate.xlsx
+++ b/src/Input/MasterTemplate.xlsx
@@ -3,19 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\invoice-generator\src\Input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ED976CC-DDB3-4791-ADB6-0816E1677677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" chartTrackingRefBase="1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures">
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
@@ -31,40 +37,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t xml:space="preserve">Owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Particulars</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HSN/SAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sq. Ft. Area</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Common Area Maintenance (CAM)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Previous Dues</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any Other  Items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total (item 1 to 5)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TOTAL AMOUNT PAYABLE BEFORE DUE DATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TERMS &amp; CONDITIONS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ACCOUNT NAME: “ESSEL TOWERS ORLOV COURT RWA “</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Post Net Banking Transfer</t>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>Particulars</t>
+  </si>
+  <si>
+    <t>HSN/SAC</t>
+  </si>
+  <si>
+    <t>Sq. Ft. Area</t>
+  </si>
+  <si>
+    <t>Common Area Maintenance (CAM)</t>
+  </si>
+  <si>
+    <t>Previous Dues</t>
+  </si>
+  <si>
+    <t>Any Other  Items</t>
+  </si>
+  <si>
+    <t>Total (item 1 to 5)</t>
+  </si>
+  <si>
+    <t>TOTAL AMOUNT PAYABLE BEFORE DUE DATE</t>
+  </si>
+  <si>
+    <t>TERMS &amp; CONDITIONS</t>
+  </si>
+  <si>
+    <t>ACCOUNT NAME: “ESSEL TOWERS ORLOV COURT RWA “</t>
+  </si>
+  <si>
+    <t>Post Net Banking Transfer</t>
   </si>
   <si>
     <r>
@@ -72,14 +78,14 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">orlovcourtrwa@</t>
+      <t>orlovcourtrwa@</t>
     </r>
     <r>
       <rPr>
@@ -89,18 +95,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">g</t>
+      <t>g</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">mail.com</t>
+      <t>mail.com</t>
     </r>
     <r>
       <rPr>
@@ -115,7 +121,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Account Payee/DD:</t>
+      <t>Account Payee/DD:</t>
     </r>
     <r>
       <rPr>
@@ -129,11 +135,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">ESSEL TOWERS ORLOV COURT RWA. </t>
@@ -146,15 +152,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Acknowledgement</t>
+      <t>Acknowledgement</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -167,12 +173,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">is subject to realization of cheque. Bank charges of Rs.500 will be payable on dishonored cheques. Outstation cheques, are required to be payable on Par in Gurugram and should be sent by courier to above mentioned ETOCRWA address. Payments above Rs.10,000/- will not be accepted in cash as per RBI Rules.</t>
+      <t>is subject to realization of cheque. Bank charges of Rs.500 will be payable on dishonored cheques. Outstation cheques, are required to be payable on Par in Gurugram and should be sent by courier to above mentioned ETOCRWA address. Payments above Rs.10,000/- will not be accepted in cash as per RBI Rules.</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Discount:</t>
+      <t>Discount:</t>
     </r>
     <r>
       <rPr>
@@ -187,7 +193,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Outstanding Dues:</t>
+      <t>Outstanding Dues:</t>
     </r>
     <r>
       <rPr>
@@ -202,7 +208,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Disputes:</t>
+      <t>Disputes:</t>
     </r>
     <r>
       <rPr>
@@ -216,11 +222,11 @@
     </r>
     <r>
       <rPr>
+        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
-        <b/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> </t>
@@ -233,95 +239,94 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">We declare this invoice shows the actual price of services described and that all particulars are true and correct.</t>
+      <t>We declare this invoice shows the actual price of services described and that all particulars are true and correct.</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">This is a system generated document and does not require a signature.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Occupant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Due Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAX-INVOICE: MAINTENANCE/CAM BILL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAN NO:   AABAE2761L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GSTIN/UIN: 06AABAE276ILIZQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Essel Towers
+    <t>This is a system generated document and does not require a signature.</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Bill Date</t>
+  </si>
+  <si>
+    <t>Bill No</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Occupant</t>
+  </si>
+  <si>
+    <t>Due Date</t>
+  </si>
+  <si>
+    <t>TAX-INVOICE: MAINTENANCE/CAM BILL</t>
+  </si>
+  <si>
+    <t>PAN NO:   AABAE2761L</t>
+  </si>
+  <si>
+    <t>GSTIN/UIN: 06AABAE276ILIZQ</t>
+  </si>
+  <si>
+    <t>Essel Towers
 Orlov Court Residents Welfare Association</t>
   </si>
   <si>
-    <t xml:space="preserve">NET BANKING-  NEFT/RTGS</t>
+    <t>NET BANKING-  NEFT/RTGS</t>
   </si>
   <si>
     <t xml:space="preserve">Bank Name:  HDFC Bank </t>
   </si>
   <si>
-    <t xml:space="preserve">Account No:  50100493615262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IFSC Code:  HDFC0009390</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sapphire Court (L-Block), Basement, Essel Towers, Main M.G. Road, Sector-28, Gurgaon – 122002, Haryana 
+    <t>Account No:  50100493615262</t>
+  </si>
+  <si>
+    <t>IFSC Code:  HDFC0009390</t>
+  </si>
+  <si>
+    <t>Sapphire Court (L-Block), Basement, Essel Towers, Main M.G. Road, Sector-28, Gurgaon – 122002, Haryana 
 Email: orlovcourtrwa@gmail.com. Tel 0124 4144748</t>
   </si>
   <si>
-    <t xml:space="preserve">Rs. Per Sq. Ft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount Payable (Rs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount (in words)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SNo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Apr'22 to June'22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Interest on Previous Dues @ 24% annum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub Total</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Round off</t>
-  </si>
-  <si>
-    <t xml:space="preserve">State Goods &amp; Services Tax @ 9%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Goods &amp; Services Tax @ 9%</t>
+    <t>Rs. Per Sq. Ft</t>
+  </si>
+  <si>
+    <t>Amount Payable (Rs)</t>
+  </si>
+  <si>
+    <t>Amount (in words)</t>
+  </si>
+  <si>
+    <t>SNo</t>
+  </si>
+  <si>
+    <t>Apr'22 to June'22</t>
+  </si>
+  <si>
+    <t>Interest on Previous Dues @ 24% annum</t>
+  </si>
+  <si>
+    <t>Sub Total</t>
+  </si>
+  <si>
+    <t>Round off</t>
+  </si>
+  <si>
+    <t>State Goods &amp; Services Tax @ 9%</t>
+  </si>
+  <si>
+    <t>Central Goods &amp; Services Tax @ 9%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -749,7 +754,7 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -819,6 +824,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -828,6 +863,111 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -836,141 +976,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,11 +984,11 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1336,11 +1341,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,93 +1358,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64"/>
-      <c r="B4" s="64"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="64"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43"/>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="43"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="73"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="74"/>
-      <c r="C7" s="74"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1462,8 +1467,8 @@
       <c r="E10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="62"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1476,10 +1481,10 @@
       <c r="E11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="27">
         <v>44658</v>
       </c>
-      <c r="G11" s="60"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1492,10 +1497,10 @@
       <c r="E12" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="57" t="s">
+      <c r="F12" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="58"/>
+      <c r="G12" s="26"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1506,10 +1511,10 @@
       <c r="E13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="70">
+      <c r="F13" s="41">
         <v>44676</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1526,10 +1531,10 @@
       <c r="A15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="43"/>
+      <c r="C15" s="55"/>
       <c r="D15" s="18" t="s">
         <v>2</v>
       </c>
@@ -1548,10 +1553,10 @@
       <c r="A16" s="15">
         <v>1</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="44"/>
+      <c r="C16" s="56"/>
       <c r="D16" s="17">
         <v>997221</v>
       </c>
@@ -1571,13 +1576,13 @@
       <c r="A17" s="15">
         <v>2</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="16">
         <v>0</v>
       </c>
@@ -1587,13 +1592,13 @@
       <c r="A18" s="15">
         <v>3</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37"/>
       <c r="G18" s="16">
         <f>IF(G17&gt;0, G17*0.24, 0)</f>
         <v>0</v>
@@ -1604,13 +1609,13 @@
       <c r="A19" s="15">
         <v>4</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37"/>
       <c r="G19" s="16">
         <v>0</v>
       </c>
@@ -1620,13 +1625,13 @@
       <c r="A20" s="15">
         <v>5</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37"/>
       <c r="G20" s="16">
         <f>SUM(G16:G19)</f>
         <v>0</v>
@@ -1637,15 +1642,15 @@
       <c r="A21" s="15">
         <v>6</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="27"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="37"/>
       <c r="G21" s="16">
-        <f>IF($G$20 &gt; 0, $G$20*0.09, 0)</f>
+        <f>IF(G20 &gt; 0, G20*0.09, 0)</f>
         <v>0</v>
       </c>
       <c r="H21" s="1"/>
@@ -1654,15 +1659,15 @@
       <c r="A22" s="15">
         <v>7</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27"/>
+      <c r="C22" s="36"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
       <c r="G22" s="16">
-        <f>IF($G$20 &gt; 0, $G$20*0.09, 0)</f>
+        <f>IF(G20 &gt; 0, G20*0.09, 0)</f>
         <v>0</v>
       </c>
       <c r="H22" s="1"/>
@@ -1671,13 +1676,13 @@
       <c r="A23" s="21">
         <v>8</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="30"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="74"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="75"/>
       <c r="G23" s="22">
         <f>SUM(G20:G22)</f>
         <v>0</v>
@@ -1688,13 +1693,13 @@
       <c r="A24" s="21">
         <v>9</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
+      <c r="C24" s="74"/>
+      <c r="D24" s="74"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="75"/>
       <c r="G24" s="16">
         <f>G25-G23</f>
         <v>0</v>
@@ -1702,14 +1707,14 @@
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:17" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="60" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="24">
         <f>ROUND(G23, 0)</f>
         <v>0</v>
@@ -1718,145 +1723,164 @@
       <c r="Q25" s="20"/>
     </row>
     <row r="26" spans="1:17" ht="14.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="55"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="68"/>
-      <c r="E26" s="68"/>
-      <c r="F26" s="68"/>
-      <c r="G26" s="69"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="38"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="40"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="63"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:17" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="47"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="55"/>
+      <c r="G28" s="59"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="B29" s="49"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="51"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="63"/>
       <c r="H29" s="1"/>
     </row>
     <row r="30" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="49"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
       <c r="G30" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="72" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="49"/>
-      <c r="C31" s="52" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="53"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="65"/>
       <c r="H31" s="1"/>
     </row>
     <row r="32" spans="1:17" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="32"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="69"/>
       <c r="H32" s="1"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="32"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="69"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:8" ht="45.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="32"/>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="34"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="69"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="35" t="s">
+      <c r="A35" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="36"/>
-      <c r="C35" s="37"/>
-      <c r="D35" s="37"/>
-      <c r="E35" s="37"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
+      <c r="B35" s="48"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="49"/>
+      <c r="F35" s="49"/>
+      <c r="G35" s="50"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B36" s="40"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
-      <c r="G36" s="42"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
+      <c r="G36" s="54"/>
       <c r="H36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="A33:G33"/>
+    <mergeCell ref="A34:G34"/>
+    <mergeCell ref="A35:G35"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="C31:G31"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="F10:G10"/>
@@ -1873,25 +1897,6 @@
     <mergeCell ref="A8:G8"/>
     <mergeCell ref="B18:F18"/>
     <mergeCell ref="B21:F21"/>
-    <mergeCell ref="A35:G35"/>
-    <mergeCell ref="A36:G36"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A29:G29"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="C31:G31"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="A33:G33"/>
-    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>